<commit_message>
Code changes for stability
</commit_message>
<xml_diff>
--- a/TestData/AmortTemplateUS - Copy.xlsx
+++ b/TestData/AmortTemplateUS - Copy.xlsx
@@ -497,12 +497,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J16"/>
+    <sheetView tabSelected="1" topLeftCell="B110" workbookViewId="0">
+      <selection sqref="A1:J129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>

</xml_diff>